<commit_message>
v0.4 - significant performance improvements.  Store piece position list in addition to board array, optimize ton of code based on profiler output
</commit_message>
<xml_diff>
--- a/Chess Performance Analysis.xlsx
+++ b/Chess Performance Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>WHITE</t>
   </si>
@@ -40,6 +40,18 @@
     <t>Time 3</t>
   </si>
   <si>
+    <t>Time 4</t>
+  </si>
+  <si>
+    <t>Time 5</t>
+  </si>
+  <si>
+    <t>Time 6</t>
+  </si>
+  <si>
+    <t>Time 7</t>
+  </si>
+  <si>
     <t>e2-e4</t>
   </si>
   <si>
@@ -166,6 +178,9 @@
     <t>e8-a8</t>
   </si>
   <si>
+    <t>0.67 *</t>
+  </si>
+  <si>
     <t>f5-f6</t>
   </si>
   <si>
@@ -178,6 +193,9 @@
     <t>h7-h6</t>
   </si>
   <si>
+    <t>1.69 **</t>
+  </si>
+  <si>
     <t>d2-g2+</t>
   </si>
   <si>
@@ -199,13 +217,37 @@
     <t>Cost vs. Time2</t>
   </si>
   <si>
-    <t>Time 1 = Basic minimax</t>
-  </si>
-  <si>
-    <t>Time 2 = Alpha Beta Pruning</t>
-  </si>
-  <si>
-    <t>Time 3 = Basic move ordering – all captures before non-captures</t>
+    <t>TOTAL thru 25</t>
+  </si>
+  <si>
+    <t>Cost vs. Time3</t>
+  </si>
+  <si>
+    <t>Cost vs. Time5</t>
+  </si>
+  <si>
+    <t>Cost vs. Time6</t>
+  </si>
+  <si>
+    <t>Time 1 = 3/16/2016 Basic minimax</t>
+  </si>
+  <si>
+    <t>Time 2 = 3/20/2016 Alpha Beta Pruning</t>
+  </si>
+  <si>
+    <t>Time 3 = 3/20/2016 Basic move ordering – all captures before non-captures</t>
+  </si>
+  <si>
+    <t>Time 4 = Sorted by capture differential – changed moves after time listed</t>
+  </si>
+  <si>
+    <t>Time 5 = Iterative Deepening, still max depth of 3.  At * computer moved e8-d7, ** computer moved d7-f5</t>
+  </si>
+  <si>
+    <t>Time 6 = Sort iterative Deepening based on expected counter if human makes expected move</t>
+  </si>
+  <si>
+    <t>Time 7 = carry piece position list around, significant improvement to move generation list</t>
   </si>
 </sst>
 </file>
@@ -306,10 +348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F39"/>
+  <dimension ref="A2:J48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -340,13 +382,25 @@
       <c r="F2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>-55</v>
@@ -360,13 +414,25 @@
       <c r="F3" s="0" t="n">
         <v>0.75</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.63</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>-90</v>
@@ -380,13 +446,25 @@
       <c r="F4" s="0" t="n">
         <v>1.91</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.49</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>-90</v>
@@ -400,13 +478,25 @@
       <c r="F5" s="0" t="n">
         <v>1.48</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>-130</v>
@@ -420,13 +510,25 @@
       <c r="F6" s="0" t="n">
         <v>3.17</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1.19</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>-115</v>
@@ -440,13 +542,25 @@
       <c r="F7" s="0" t="n">
         <v>1.7</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>-100</v>
@@ -460,13 +574,25 @@
       <c r="F8" s="0" t="n">
         <v>1.66</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.57</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>-120</v>
@@ -480,13 +606,25 @@
       <c r="F9" s="0" t="n">
         <v>3.24</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>-55</v>
@@ -500,13 +638,25 @@
       <c r="F10" s="0" t="n">
         <v>2.08</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>-45</v>
@@ -520,13 +670,25 @@
       <c r="F11" s="0" t="n">
         <v>2.49</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>-10</v>
@@ -540,13 +702,22 @@
       <c r="F12" s="0" t="n">
         <v>1.77</v>
       </c>
+      <c r="H12" s="0" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>315</v>
@@ -560,13 +731,22 @@
       <c r="F13" s="0" t="n">
         <v>2.48</v>
       </c>
+      <c r="H13" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0.62</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>90</v>
@@ -580,13 +760,22 @@
       <c r="F14" s="0" t="n">
         <v>1.92</v>
       </c>
+      <c r="H14" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0.57</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>-105</v>
@@ -600,13 +789,22 @@
       <c r="F15" s="0" t="n">
         <v>1.68</v>
       </c>
+      <c r="H15" s="0" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0.82</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>95</v>
@@ -620,13 +818,22 @@
       <c r="F16" s="0" t="n">
         <v>1.89</v>
       </c>
+      <c r="H16" s="0" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0.83</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>165</v>
@@ -640,13 +847,22 @@
       <c r="F17" s="0" t="n">
         <v>1.08</v>
       </c>
+      <c r="H17" s="0" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0.57</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>155</v>
@@ -660,13 +876,22 @@
       <c r="F18" s="0" t="n">
         <v>1.28</v>
       </c>
+      <c r="H18" s="0" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0.63</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>325</v>
@@ -680,13 +905,22 @@
       <c r="F19" s="0" t="n">
         <v>0.86</v>
       </c>
+      <c r="H19" s="0" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>325</v>
@@ -700,13 +934,22 @@
       <c r="F20" s="0" t="n">
         <v>0.91</v>
       </c>
+      <c r="H20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>310</v>
@@ -720,13 +963,22 @@
       <c r="F21" s="0" t="n">
         <v>1.46</v>
       </c>
+      <c r="H21" s="0" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>335</v>
@@ -740,13 +992,22 @@
       <c r="F22" s="0" t="n">
         <v>1.22</v>
       </c>
+      <c r="H22" s="0" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0.57</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>655</v>
@@ -760,13 +1021,22 @@
       <c r="F23" s="0" t="n">
         <v>0.73</v>
       </c>
+      <c r="H23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>645</v>
@@ -780,13 +1050,22 @@
       <c r="F24" s="0" t="n">
         <v>0.62</v>
       </c>
+      <c r="H24" s="0" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0.55</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>805</v>
@@ -800,13 +1079,22 @@
       <c r="F25" s="0" t="n">
         <v>0.87</v>
       </c>
+      <c r="H25" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>1.11</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>100001</v>
@@ -823,15 +1111,15 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">SUM(D3:D26)</f>
@@ -848,7 +1136,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="false">E29/D29</f>
@@ -861,7 +1149,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="n">
@@ -869,19 +1157,173 @@
         <v>0.190149435803599</v>
       </c>
     </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">SUM(D3:D25)</f>
+        <v>725.49</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <f aca="false">SUM(E3:E25)</f>
+        <v>196.46</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <f aca="false">SUM(F3:F25)</f>
+        <v>37.25</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <f aca="false">SUM(H3:H25) + 0.67 + 1.69</f>
+        <v>33.43</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <f aca="false">SUM(I3:I25)</f>
+        <v>33.68</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f aca="false">SUM(J3:J25)</f>
+        <v>16.31</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="n">
+        <f aca="false">E33/$D$33</f>
+        <v>0.270796289404403</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <f aca="false">F33/$D$33</f>
+        <v>0.0513446084715158</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="n">
+        <f aca="false">H33/$D$33</f>
+        <v>0.0460792016430275</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <f aca="false">I33/$D$33</f>
+        <v>0.0464237963307558</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <f aca="false">J33/$D$33</f>
+        <v>0.0224813574273939</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="n">
+        <f aca="false">F33/$E$33</f>
+        <v>0.189606026672096</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="n">
+        <f aca="false">H33/$E$33</f>
+        <v>0.170161865010689</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <f aca="false">I33/$E$33</f>
+        <v>0.171434388679629</v>
+      </c>
+      <c r="J35" s="1" t="n">
+        <f aca="false">J33/$E$33</f>
+        <v>0.0830194441616614</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="n">
+        <f aca="false">H33/$F$33</f>
+        <v>0.89744966442953</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <f aca="false">I33/$F$33</f>
+        <v>0.904161073825503</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <f aca="false">J33/$F$33</f>
+        <v>0.437852348993289</v>
+      </c>
+    </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="n">
+        <f aca="false">I33/$H$33</f>
+        <v>1.00747831289261</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <f aca="false">J33/$H$33</f>
+        <v>0.48788513311397</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1" t="n">
+        <f aca="false">J33/I33</f>
+        <v>0.484263657957245</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v 0.5 - added board caching to improve move calculation speed
</commit_message>
<xml_diff>
--- a/Chess Performance Analysis.xlsx
+++ b/Chess Performance Analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>WHITE</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Time 7</t>
   </si>
   <si>
+    <t>Time 8</t>
+  </si>
+  <si>
     <t>e2-e4</t>
   </si>
   <si>
@@ -248,6 +251,9 @@
   </si>
   <si>
     <t>Time 7 = carry piece position list around, significant improvement to move generation list</t>
+  </si>
+  <si>
+    <t>Time 8 = added transposition table / move cache</t>
   </si>
 </sst>
 </file>
@@ -263,6 +269,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -348,19 +355,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J48"/>
+  <dimension ref="A2:K49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.64285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.91836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.68367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.98469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.80612244897959"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.77551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.08163265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.21938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,13 +408,16 @@
       <c r="J2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>-55</v>
@@ -426,13 +443,16 @@
       <c r="J3" s="0" t="n">
         <v>0.63</v>
       </c>
+      <c r="K3" s="0" t="n">
+        <v>0.59</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>-90</v>
@@ -458,13 +478,16 @@
       <c r="J4" s="0" t="n">
         <v>0.49</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>-90</v>
@@ -490,13 +513,16 @@
       <c r="J5" s="0" t="n">
         <v>0.54</v>
       </c>
+      <c r="K5" s="0" t="n">
+        <v>0.56</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>-130</v>
@@ -522,13 +548,16 @@
       <c r="J6" s="0" t="n">
         <v>1.19</v>
       </c>
+      <c r="K6" s="0" t="n">
+        <v>1.18</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>-115</v>
@@ -554,13 +583,16 @@
       <c r="J7" s="0" t="n">
         <v>0.89</v>
       </c>
+      <c r="K7" s="0" t="n">
+        <v>0.86</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>-100</v>
@@ -586,13 +618,16 @@
       <c r="J8" s="0" t="n">
         <v>0.57</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <v>0.55</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>-120</v>
@@ -618,13 +653,16 @@
       <c r="J9" s="0" t="n">
         <v>1.5</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <v>1.52</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>-55</v>
@@ -650,13 +688,16 @@
       <c r="J10" s="0" t="n">
         <v>0.68</v>
       </c>
+      <c r="K10" s="0" t="n">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>-45</v>
@@ -682,13 +723,16 @@
       <c r="J11" s="0" t="n">
         <v>0.71</v>
       </c>
+      <c r="K11" s="0" t="n">
+        <v>0.72</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>-10</v>
@@ -714,10 +758,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>315</v>
@@ -743,10 +787,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>90</v>
@@ -772,10 +816,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>-105</v>
@@ -801,10 +845,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>95</v>
@@ -830,10 +874,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>165</v>
@@ -859,10 +903,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>155</v>
@@ -888,10 +932,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>325</v>
@@ -917,10 +961,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>325</v>
@@ -946,10 +990,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>310</v>
@@ -975,10 +1019,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>335</v>
@@ -1004,10 +1048,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>655</v>
@@ -1022,7 +1066,7 @@
         <v>0.73</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>0.69</v>
@@ -1033,10 +1077,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>645</v>
@@ -1062,10 +1106,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>805</v>
@@ -1080,7 +1124,7 @@
         <v>0.87</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>1.74</v>
@@ -1091,10 +1135,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>100001</v>
@@ -1111,15 +1155,15 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">SUM(D3:D26)</f>
@@ -1136,7 +1180,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="false">E29/D29</f>
@@ -1149,7 +1193,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="n">
@@ -1159,7 +1203,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D33" s="0" t="n">
         <f aca="false">SUM(D3:D25)</f>
@@ -1188,7 +1232,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="n">
@@ -1215,7 +1259,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1239,7 +1283,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1260,7 +1304,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1278,7 +1322,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1293,37 +1337,42 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>